<commit_message>
MVC UPDATED PEMBAYAN SPP DAN KJP
</commit_message>
<xml_diff>
--- a/temp_doc/DATA KELAS FIX.xlsx
+++ b/temp_doc/DATA KELAS FIX.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/sppth_terbaru/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{716446F8-0C8B-504E-AD3D-CC42FE08D422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B12F37-2D81-E54F-9889-3AFDDF2A3075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="2260" windowWidth="27240" windowHeight="15940" xr2:uid="{AB72E732-1B4D-0449-8A67-D584FA100D85}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{AB72E732-1B4D-0449-8A67-D584FA100D85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>XII TKJ 3</t>
+  </si>
+  <si>
+    <t>X DKV 1</t>
+  </si>
+  <si>
+    <t>DKV</t>
   </si>
 </sst>
 </file>
@@ -188,10 +194,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,15 +513,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664577AF-41FC-0C49-BD7B-86162BAED619}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:D54"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +537,17 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1">
+        <v>101</v>
+      </c>
+      <c r="F1">
+        <v>202</v>
+      </c>
+      <c r="G1">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001520</v>
       </c>
@@ -541,8 +560,20 @@
       <c r="D2">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <f>COUNTIF(D2:D80,E1)</f>
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(D2:D80,F1)</f>
+        <v>26</v>
+      </c>
+      <c r="G2">
+        <f>COUNTIF(D2:D80,G1)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002382</v>
       </c>
@@ -556,7 +587,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003282</v>
       </c>
@@ -570,7 +601,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004737</v>
       </c>
@@ -584,7 +615,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005348</v>
       </c>
@@ -598,7 +629,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006846</v>
       </c>
@@ -612,7 +643,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007627</v>
       </c>
@@ -626,7 +657,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008602</v>
       </c>
@@ -640,7 +671,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009189</v>
       </c>
@@ -654,7 +685,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1010805</v>
       </c>
@@ -668,7 +699,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1011905</v>
       </c>
@@ -682,7 +713,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1012396</v>
       </c>
@@ -696,7 +727,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1013157</v>
       </c>
@@ -710,7 +741,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1014691</v>
       </c>
@@ -724,7 +755,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1015808</v>
       </c>
@@ -1268,6 +1299,370 @@
       </c>
       <c r="D54">
         <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>3035146</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>3037075</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>3031535</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>3033468</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>3037072</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>3032783</v>
+      </c>
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>3035345</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>3035241</v>
+      </c>
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>3035294</v>
+      </c>
+      <c r="B63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>3035455</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>3031564</v>
+      </c>
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
+        <v>3033800</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D66">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>3031131</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>3034929</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>3039219</v>
+      </c>
+      <c r="B69" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>3039924</v>
+      </c>
+      <c r="B70" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
+        <v>3032709</v>
+      </c>
+      <c r="B71" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
+        <v>3031901</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
+        <v>3035387</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D73">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>3037487</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>3031557</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>3035861</v>
+      </c>
+      <c r="B76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
+        <v>3039274</v>
+      </c>
+      <c r="B77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="3">
+        <v>3031974</v>
+      </c>
+      <c r="B78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D78">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="3">
+        <v>3031195</v>
+      </c>
+      <c r="B79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
+        <v>3036135</v>
+      </c>
+      <c r="B80" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D80">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MVS UPDATE DATS PEMBAYARAN
</commit_message>
<xml_diff>
--- a/temp_doc/DATA KELAS FIX.xlsx
+++ b/temp_doc/DATA KELAS FIX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/sppth_terbaru/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B12F37-2D81-E54F-9889-3AFDDF2A3075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949430C5-2B38-844F-8D8B-5EBD8E31949A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{AB72E732-1B4D-0449-8A67-D584FA100D85}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{AB72E732-1B4D-0449-8A67-D584FA100D85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,94 +58,94 @@
     <t>X AKL 2</t>
   </si>
   <si>
-    <t>BDP</t>
-  </si>
-  <si>
-    <t>X BDP 1</t>
-  </si>
-  <si>
-    <t>X BDP 2</t>
-  </si>
-  <si>
-    <t>OTKP</t>
-  </si>
-  <si>
-    <t>X OTKP 1</t>
-  </si>
-  <si>
-    <t>X OTKP 2</t>
-  </si>
-  <si>
-    <t>TKJ</t>
-  </si>
-  <si>
-    <t>X TKJ 1</t>
-  </si>
-  <si>
-    <t>X TKJ 2</t>
-  </si>
-  <si>
-    <t>X TKJ 3</t>
-  </si>
-  <si>
     <t>XI AKL 1</t>
   </si>
   <si>
     <t>XI AKL 2</t>
   </si>
   <si>
-    <t>XI BDP 1</t>
-  </si>
-  <si>
-    <t>XI BDP 2</t>
-  </si>
-  <si>
-    <t>XI OTKP 1</t>
-  </si>
-  <si>
-    <t>XI OTKP 2</t>
-  </si>
-  <si>
-    <t>XI TKJ 1</t>
-  </si>
-  <si>
-    <t>XI TKJ 2</t>
-  </si>
-  <si>
-    <t>XI TKJ 3</t>
-  </si>
-  <si>
     <t>XII AKL 1</t>
   </si>
   <si>
     <t>XII AKL 2</t>
   </si>
   <si>
-    <t>XII BDP 1</t>
-  </si>
-  <si>
-    <t>XII BDP 2</t>
-  </si>
-  <si>
-    <t>XII OTKP 1</t>
-  </si>
-  <si>
-    <t>XII OTKP 2</t>
-  </si>
-  <si>
-    <t>XII TKJ 1</t>
-  </si>
-  <si>
-    <t>XII TKJ 2</t>
-  </si>
-  <si>
-    <t>XII TKJ 3</t>
-  </si>
-  <si>
     <t>X DKV 1</t>
   </si>
   <si>
     <t>DKV</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>X PM 1</t>
+  </si>
+  <si>
+    <t>X PM 2</t>
+  </si>
+  <si>
+    <t>XI PM 1</t>
+  </si>
+  <si>
+    <t>XI PM 2</t>
+  </si>
+  <si>
+    <t>XII PM 1</t>
+  </si>
+  <si>
+    <t>XII PM 2</t>
+  </si>
+  <si>
+    <t>MPLB</t>
+  </si>
+  <si>
+    <t>X MPLB 1</t>
+  </si>
+  <si>
+    <t>X MPLB 2</t>
+  </si>
+  <si>
+    <t>XI MPLB 1</t>
+  </si>
+  <si>
+    <t>XI MPLB 2</t>
+  </si>
+  <si>
+    <t>XII MPLB 1</t>
+  </si>
+  <si>
+    <t>XII MPLB 2</t>
+  </si>
+  <si>
+    <t>TJKT</t>
+  </si>
+  <si>
+    <t>X TJKT 1</t>
+  </si>
+  <si>
+    <t>X TJKT 2</t>
+  </si>
+  <si>
+    <t>X TJKT 3</t>
+  </si>
+  <si>
+    <t>XI TJKT 1</t>
+  </si>
+  <si>
+    <t>XI TJKT 2</t>
+  </si>
+  <si>
+    <t>XI TJKT 3</t>
+  </si>
+  <si>
+    <t>XII TJKT 1</t>
+  </si>
+  <si>
+    <t>XII TJKT 2</t>
+  </si>
+  <si>
+    <t>XII TJKT 3</t>
   </si>
 </sst>
 </file>
@@ -194,11 +194,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,7 +216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -505,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664577AF-41FC-0C49-BD7B-86162BAED619}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +523,7 @@
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,17 +536,8 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1">
-        <v>101</v>
-      </c>
-      <c r="F1">
-        <v>202</v>
-      </c>
-      <c r="G1">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001520</v>
       </c>
@@ -560,20 +550,8 @@
       <c r="D2">
         <v>101</v>
       </c>
-      <c r="E2">
-        <f>COUNTIF(D2:D80,E1)</f>
-        <v>27</v>
-      </c>
-      <c r="F2">
-        <f>COUNTIF(D2:D80,F1)</f>
-        <v>26</v>
-      </c>
-      <c r="G2">
-        <f>COUNTIF(D2:D80,G1)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002382</v>
       </c>
@@ -587,105 +565,105 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003282</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004737</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005348</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006846</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D7">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007627</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008602</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009189</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1010805</v>
       </c>
@@ -693,13 +671,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1011905</v>
       </c>
@@ -707,63 +685,63 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1012396</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1013157</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1014691</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D15">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1015808</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <v>101</v>
@@ -774,10 +752,10 @@
         <v>1016934</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>101</v>
@@ -788,10 +766,10 @@
         <v>1017641</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D18">
         <v>101</v>
@@ -802,10 +780,10 @@
         <v>1018307</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>101</v>
@@ -819,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>101</v>
@@ -833,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D21">
         <v>101</v>
@@ -844,10 +822,10 @@
         <v>1021281</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D22">
         <v>101</v>
@@ -858,10 +836,10 @@
         <v>1022954</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D23">
         <v>101</v>
@@ -872,10 +850,10 @@
         <v>1023249</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D24">
         <v>101</v>
@@ -886,10 +864,10 @@
         <v>1024545</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D25">
         <v>101</v>
@@ -900,10 +878,10 @@
         <v>1025447</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D26">
         <v>101</v>
@@ -914,10 +892,10 @@
         <v>1026779</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D27">
         <v>101</v>
@@ -928,10 +906,10 @@
         <v>1027111</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D28">
         <v>101</v>
@@ -970,10 +948,10 @@
         <v>2004629</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D31">
         <v>202</v>
@@ -984,10 +962,10 @@
         <v>2005641</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D32">
         <v>202</v>
@@ -998,10 +976,10 @@
         <v>2006284</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D33">
         <v>202</v>
@@ -1012,10 +990,10 @@
         <v>2007982</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D34">
         <v>202</v>
@@ -1026,10 +1004,10 @@
         <v>2008874</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D35">
         <v>202</v>
@@ -1040,10 +1018,10 @@
         <v>2009657</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D36">
         <v>202</v>
@@ -1057,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D37">
         <v>202</v>
@@ -1071,7 +1049,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D38">
         <v>202</v>
@@ -1082,10 +1060,10 @@
         <v>2012891</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D39">
         <v>202</v>
@@ -1096,10 +1074,10 @@
         <v>2013872</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D40">
         <v>202</v>
@@ -1110,10 +1088,10 @@
         <v>2014732</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D41">
         <v>202</v>
@@ -1124,10 +1102,10 @@
         <v>2015323</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D42">
         <v>202</v>
@@ -1138,10 +1116,10 @@
         <v>2016903</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D43">
         <v>202</v>
@@ -1152,10 +1130,10 @@
         <v>2017942</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D44">
         <v>202</v>
@@ -1166,10 +1144,10 @@
         <v>2018897</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D45">
         <v>202</v>
@@ -1183,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D46">
         <v>202</v>
@@ -1197,7 +1175,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D47">
         <v>202</v>
@@ -1208,10 +1186,10 @@
         <v>2021970</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D48">
         <v>202</v>
@@ -1222,10 +1200,10 @@
         <v>2022257</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D49">
         <v>202</v>
@@ -1236,10 +1214,10 @@
         <v>2023991</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D50">
         <v>202</v>
@@ -1250,10 +1228,10 @@
         <v>2024974</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D51">
         <v>202</v>
@@ -1264,10 +1242,10 @@
         <v>2025238</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D52">
         <v>202</v>
@@ -1278,10 +1256,10 @@
         <v>2026164</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D53">
         <v>202</v>
@@ -1292,17 +1270,17 @@
         <v>2027903</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D54">
         <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
+      <c r="A55">
         <v>3035146</v>
       </c>
       <c r="B55" t="s">
@@ -1316,7 +1294,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="3">
+      <c r="A56">
         <v>3037075</v>
       </c>
       <c r="B56" t="s">
@@ -1330,336 +1308,336 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="3">
+      <c r="A57">
         <v>3031535</v>
       </c>
       <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>3033468</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>3037072</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>3032783</v>
+      </c>
+      <c r="B60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D60">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>3035345</v>
+      </c>
+      <c r="B61" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>3035241</v>
+      </c>
+      <c r="B62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>3035294</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>3035455</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
         <v>7</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D64">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>3031564</v>
+      </c>
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D57">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
-        <v>3033468</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="D65">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>3033800</v>
+      </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>3031131</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>3034929</v>
+      </c>
+      <c r="B68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>3039219</v>
+      </c>
+      <c r="B69" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>3039924</v>
+      </c>
+      <c r="B70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>3032709</v>
+      </c>
+      <c r="B71" t="s">
+        <v>27</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>3031901</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>3035387</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
-        <v>3037072</v>
-      </c>
-      <c r="B59" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
-        <v>3032783</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="D73">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>3037487</v>
+      </c>
+      <c r="B74" t="s">
         <v>13</v>
       </c>
-      <c r="C60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
-        <v>3035345</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>3031557</v>
+      </c>
+      <c r="B75" t="s">
         <v>13</v>
       </c>
-      <c r="C61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
-        <v>3035241</v>
-      </c>
-      <c r="B62" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
-        <v>3035294</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C75" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>3035861</v>
+      </c>
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D76">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>3039274</v>
+      </c>
+      <c r="B77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>3031974</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>3031195</v>
+      </c>
+      <c r="B79" t="s">
+        <v>27</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>3036135</v>
+      </c>
+      <c r="B80" t="s">
+        <v>27</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C63" t="s">
-        <v>35</v>
-      </c>
-      <c r="D63">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
-        <v>3035455</v>
-      </c>
-      <c r="B64" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" t="s">
-        <v>17</v>
-      </c>
-      <c r="D64">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
-        <v>3031564</v>
-      </c>
-      <c r="B65" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="3">
-        <v>3033800</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D66">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="3">
-        <v>3031131</v>
-      </c>
-      <c r="B67" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="3">
-        <v>3034929</v>
-      </c>
-      <c r="B68" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D68">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="3">
-        <v>3039219</v>
-      </c>
-      <c r="B69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
-        <v>3039924</v>
-      </c>
-      <c r="B70" t="s">
-        <v>13</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D70">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="3">
-        <v>3032709</v>
-      </c>
-      <c r="B71" t="s">
-        <v>13</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D71">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="3">
-        <v>3031901</v>
-      </c>
-      <c r="B72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D72">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="3">
-        <v>3035387</v>
-      </c>
-      <c r="B73" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D73">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="3">
-        <v>3037487</v>
-      </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D74">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="3">
-        <v>3031557</v>
-      </c>
-      <c r="B75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="3">
-        <v>3035861</v>
-      </c>
-      <c r="B76" t="s">
-        <v>10</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D76">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="3">
-        <v>3039274</v>
-      </c>
-      <c r="B77" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D77">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="3">
-        <v>3031974</v>
-      </c>
-      <c r="B78" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D78">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="3">
-        <v>3031195</v>
-      </c>
-      <c r="B79" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D79">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="3">
-        <v>3036135</v>
-      </c>
-      <c r="B80" t="s">
-        <v>13</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D80">
         <v>303</v>

</xml_diff>

<commit_message>
MVC UPDATE PEMBAYARAN PER NIS
</commit_message>
<xml_diff>
--- a/temp_doc/DATA KELAS FIX.xlsx
+++ b/temp_doc/DATA KELAS FIX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/sppth_terbaru/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85846F20-C8ED-1F4A-8A2E-F9462D9225E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8F9B06-A5E5-B54F-8088-8570833C548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{AB72E732-1B4D-0449-8A67-D584FA100D85}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
   <si>
     <t>id</t>
   </si>
@@ -188,10 +188,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664577AF-41FC-0C49-BD7B-86162BAED619}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,8 +533,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>3035146</v>
+      <c r="A2" s="3">
+        <v>10001303</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -546,8 +547,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>3037075</v>
+      <c r="A3" s="3">
+        <v>10002303</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -560,8 +561,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3031535</v>
+      <c r="A4" s="3">
+        <v>10003303</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -574,8 +575,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3033468</v>
+      <c r="A5" s="3">
+        <v>10004303</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -588,8 +589,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3037072</v>
+      <c r="A6" s="3">
+        <v>10005303</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -602,8 +603,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3032783</v>
+      <c r="A7" s="3">
+        <v>10006303</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -616,8 +617,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3035345</v>
+      <c r="A8" s="3">
+        <v>10007303</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -630,8 +631,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>3035241</v>
+      <c r="A9" s="3">
+        <v>10008303</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -644,8 +645,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>3035294</v>
+      <c r="A10" s="3">
+        <v>10009303</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -658,8 +659,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>3035455</v>
+      <c r="A11" s="3">
+        <v>10010303</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -672,8 +673,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>3031564</v>
+      <c r="A12" s="3">
+        <v>10011303</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -686,8 +687,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>3033800</v>
+      <c r="A13" s="3">
+        <v>10012303</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -700,8 +701,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>3031131</v>
+      <c r="A14" s="3">
+        <v>10013303</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -714,8 +715,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>3034929</v>
+      <c r="A15" s="3">
+        <v>10014303</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -728,8 +729,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>3039219</v>
+      <c r="A16" s="3">
+        <v>10015303</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -742,8 +743,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>3039924</v>
+      <c r="A17" s="3">
+        <v>10016303</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -756,8 +757,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>3032709</v>
+      <c r="A18" s="3">
+        <v>10017303</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
@@ -770,8 +771,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>3031901</v>
+      <c r="A19" s="3">
+        <v>10018303</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -784,8 +785,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>3035387</v>
+      <c r="A20" s="3">
+        <v>10019303</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -798,8 +799,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>3037487</v>
+      <c r="A21" s="3">
+        <v>10020303</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
@@ -812,8 +813,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>3031557</v>
+      <c r="A22" s="3">
+        <v>10021303</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
@@ -826,8 +827,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>3035861</v>
+      <c r="A23" s="3">
+        <v>10022303</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
@@ -840,8 +841,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>3039274</v>
+      <c r="A24" s="3">
+        <v>10023303</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -854,8 +855,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>3031974</v>
+      <c r="A25" s="3">
+        <v>10024303</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -868,8 +869,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>3031195</v>
+      <c r="A26" s="3">
+        <v>10025303</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -882,8 +883,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>3036135</v>
+      <c r="A27" s="3">
+        <v>10026303</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -893,6 +894,370 @@
       </c>
       <c r="D27">
         <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>10027404</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>10028404</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>10029404</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>10030404</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>10031404</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>10032404</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>10033404</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>10034404</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>10035404</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>10036404</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>10037404</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>10038404</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>10039404</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>10040404</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>10041404</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>10042404</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>10043404</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>10044404</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>10045404</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>10046404</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>10047404</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>10048404</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>10049404</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>10050404</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>10051404</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>10052404</v>
+      </c>
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53">
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MVC UPDATE SETTING SPP
</commit_message>
<xml_diff>
--- a/temp_doc/DATA KELAS FIX.xlsx
+++ b/temp_doc/DATA KELAS FIX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/sppth_terbaru/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F6D667-5722-694E-8E84-1B0FEF49AB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF96570-7C80-2A49-BD3A-7B1BF5D44A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{AB72E732-1B4D-0449-8A67-D584FA100D85}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -145,7 +145,10 @@
     <t>XI DKV</t>
   </si>
   <si>
-    <t>XI PM</t>
+    <t xml:space="preserve">XI PM </t>
+  </si>
+  <si>
+    <t>XII PM</t>
   </si>
 </sst>
 </file>
@@ -174,12 +177,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -194,11 +203,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664577AF-41FC-0C49-BD7B-86162BAED619}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +536,7 @@
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,8 +550,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>1001303</v>
       </c>
       <c r="B2" t="s">
@@ -551,9 +563,16 @@
       <c r="D2">
         <v>303</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="E2">
+        <v>1001</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(E2,D2)</f>
+        <v>1001303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>1002303</v>
       </c>
       <c r="B3" t="s">
@@ -565,9 +584,16 @@
       <c r="D3">
         <v>303</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="E3">
+        <v>1002</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F53" si="0">_xlfn.CONCAT(E3,D3)</f>
+        <v>1002303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>1003303</v>
       </c>
       <c r="B4" t="s">
@@ -579,9 +605,16 @@
       <c r="D4">
         <v>303</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="E4">
+        <v>1003</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>1003303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>1004303</v>
       </c>
       <c r="B5" t="s">
@@ -593,9 +626,16 @@
       <c r="D5">
         <v>303</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="E5">
+        <v>1004</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>1004303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>1005303</v>
       </c>
       <c r="B6" t="s">
@@ -607,9 +647,16 @@
       <c r="D6">
         <v>303</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="E6">
+        <v>1005</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>1005303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>1006303</v>
       </c>
       <c r="B7" t="s">
@@ -621,9 +668,16 @@
       <c r="D7">
         <v>303</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="E7">
+        <v>1006</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>1006303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>1007303</v>
       </c>
       <c r="B8" t="s">
@@ -635,9 +689,16 @@
       <c r="D8">
         <v>303</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="E8">
+        <v>1007</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>1007303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>1008303</v>
       </c>
       <c r="B9" t="s">
@@ -649,9 +710,16 @@
       <c r="D9">
         <v>303</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="E9">
+        <v>1008</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>1008303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>1009303</v>
       </c>
       <c r="B10" t="s">
@@ -663,9 +731,16 @@
       <c r="D10">
         <v>303</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="E10">
+        <v>1009</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>1009303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>1010303</v>
       </c>
       <c r="B11" t="s">
@@ -677,9 +752,16 @@
       <c r="D11">
         <v>303</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="E11">
+        <v>1010</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>1010303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>1011303</v>
       </c>
       <c r="B12" t="s">
@@ -691,9 +773,16 @@
       <c r="D12">
         <v>303</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="E12">
+        <v>1011</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>1011303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>1012303</v>
       </c>
       <c r="B13" t="s">
@@ -705,9 +794,16 @@
       <c r="D13">
         <v>303</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="E13">
+        <v>1012</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>1012303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>1013303</v>
       </c>
       <c r="B14" t="s">
@@ -719,9 +815,16 @@
       <c r="D14">
         <v>303</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="E14">
+        <v>1013</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>1013303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>1014303</v>
       </c>
       <c r="B15" t="s">
@@ -733,9 +836,16 @@
       <c r="D15">
         <v>303</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="E15">
+        <v>1014</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>1014303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>1015303</v>
       </c>
       <c r="B16" t="s">
@@ -747,9 +857,16 @@
       <c r="D16">
         <v>303</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="E16">
+        <v>1015</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>1015303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>1016303</v>
       </c>
       <c r="B17" t="s">
@@ -761,9 +878,16 @@
       <c r="D17">
         <v>303</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="E17">
+        <v>1016</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>1016303</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
         <v>1017303</v>
       </c>
       <c r="B18" t="s">
@@ -775,9 +899,16 @@
       <c r="D18">
         <v>303</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="E18">
+        <v>1017</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>1017303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
         <v>1018303</v>
       </c>
       <c r="B19" t="s">
@@ -789,9 +920,16 @@
       <c r="D19">
         <v>303</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="E19">
+        <v>1018</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>1018303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
         <v>1019303</v>
       </c>
       <c r="B20" t="s">
@@ -803,9 +941,16 @@
       <c r="D20">
         <v>303</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="E20">
+        <v>1019</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>1019303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
         <v>1020303</v>
       </c>
       <c r="B21" t="s">
@@ -817,9 +962,16 @@
       <c r="D21">
         <v>303</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="E21">
+        <v>1020</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>1020303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>1021303</v>
       </c>
       <c r="B22" t="s">
@@ -831,9 +983,16 @@
       <c r="D22">
         <v>303</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="E22">
+        <v>1021</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>1021303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
         <v>1022303</v>
       </c>
       <c r="B23" t="s">
@@ -845,9 +1004,16 @@
       <c r="D23">
         <v>303</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="E23">
+        <v>1022</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>1022303</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>1023303</v>
       </c>
       <c r="B24" t="s">
@@ -859,9 +1025,16 @@
       <c r="D24">
         <v>303</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="E24">
+        <v>1023</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>1023303</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
         <v>1024303</v>
       </c>
       <c r="B25" t="s">
@@ -873,9 +1046,16 @@
       <c r="D25">
         <v>303</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="E25">
+        <v>1024</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>1024303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
         <v>1025303</v>
       </c>
       <c r="B26" t="s">
@@ -887,312 +1067,585 @@
       <c r="D26">
         <v>303</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="E26">
+        <v>1025</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>1025303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
         <v>1026303</v>
       </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D27">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="D27" s="3">
+        <v>303</v>
+      </c>
+      <c r="E27">
+        <v>1026</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>1026303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
         <v>1027404</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>33</v>
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
       </c>
       <c r="D28">
         <v>404</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="E28">
+        <v>1027</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>1027404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
         <v>1028404</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29">
         <v>404</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="E29">
+        <v>1028</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>1028404</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
         <v>1029404</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
       </c>
       <c r="D30">
         <v>404</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="E30">
+        <v>1029</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>1029404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
         <v>1030404</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
       </c>
       <c r="D31">
         <v>404</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="E31">
+        <v>1030</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>1030404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
         <v>1031404</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>19</v>
+      <c r="C32" t="s">
+        <v>18</v>
       </c>
       <c r="D32">
         <v>404</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="E32">
+        <v>1031</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>1031404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
         <v>1032404</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
       </c>
       <c r="D33">
         <v>404</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="E33">
+        <v>1032</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>1032404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
         <v>1033404</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>27</v>
+      <c r="C34" t="s">
+        <v>25</v>
       </c>
       <c r="D34">
         <v>404</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="E34">
+        <v>1033</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>1033404</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
         <v>1034404</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>28</v>
+      <c r="C35" t="s">
+        <v>26</v>
       </c>
       <c r="D35">
         <v>404</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="E35">
+        <v>1034</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>1034404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
         <v>1035404</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
       </c>
       <c r="D36">
         <v>404</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+      <c r="E36">
+        <v>1035</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>1035404</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
         <v>1036404</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
       </c>
       <c r="D37">
         <v>404</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+      <c r="E37">
+        <v>1036</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>1036404</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <v>1037404</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>404</v>
+      </c>
+      <c r="E38">
+        <v>1037</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>1037404</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>1038404</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39">
+        <v>404</v>
+      </c>
+      <c r="E39">
+        <v>1038</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>1038404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>1039404</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40">
+        <v>404</v>
+      </c>
+      <c r="E40">
+        <v>1039</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>1039404</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>1040404</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41">
+        <v>404</v>
+      </c>
+      <c r="E41">
+        <v>1040</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>1040404</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>1041404</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42">
+        <v>404</v>
+      </c>
+      <c r="E42">
+        <v>1041</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>1041404</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>1042404</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43">
+        <v>404</v>
+      </c>
+      <c r="E43">
+        <v>1042</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>1042404</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>1043404</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44">
+        <v>404</v>
+      </c>
+      <c r="E44">
+        <v>1043</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>1043404</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>1044404</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45">
+        <v>404</v>
+      </c>
+      <c r="E45">
+        <v>1044</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>1044404</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>1045404</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D38">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
-        <v>1038404</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D46">
+        <v>404</v>
+      </c>
+      <c r="E46">
+        <v>1045</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>1045404</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>1046404</v>
+      </c>
+      <c r="B47" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D39">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
-        <v>1039404</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="D47">
+        <v>404</v>
+      </c>
+      <c r="E47">
+        <v>1046</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>1046404</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>1047404</v>
+      </c>
+      <c r="B48" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
-        <v>1040404</v>
-      </c>
-      <c r="B41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
-        <v>1041404</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C48" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48">
+        <v>404</v>
+      </c>
+      <c r="E48">
+        <v>1047</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>1047404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>1048404</v>
+      </c>
+      <c r="B49" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D42">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
-        <v>1042404</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="D49">
+        <v>404</v>
+      </c>
+      <c r="E49">
+        <v>1048</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>1048404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>1049404</v>
+      </c>
+      <c r="B50" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D43">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
-        <v>1043404</v>
-      </c>
-      <c r="B44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="D50">
+        <v>404</v>
+      </c>
+      <c r="E50">
+        <v>1049</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>1049404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>1050404</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D44">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
-        <v>1044404</v>
-      </c>
-      <c r="B45" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="D51">
+        <v>404</v>
+      </c>
+      <c r="E51">
+        <v>1050</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>1050404</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>1051404</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D45">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
-        <v>1045404</v>
-      </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="D52">
+        <v>404</v>
+      </c>
+      <c r="E52">
+        <v>1051</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>1051404</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>1052404</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D46">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>404</v>
+      </c>
+      <c r="E53">
+        <v>1052</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>1052404</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C55" s="2"/>
     </row>
   </sheetData>

</xml_diff>